<commit_message>
fix: remove preparent_item_1_id in item_id: 2
</commit_message>
<xml_diff>
--- a/master_data.xlsx
+++ b/master_data.xlsx
@@ -1438,9 +1438,7 @@
       <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="3">
-        <v>1</v>
-      </c>
+      <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>

</xml_diff>

<commit_message>
add opening master xlsx
</commit_message>
<xml_diff>
--- a/master_data.xlsx
+++ b/master_data.xlsx
@@ -6,12 +6,13 @@
   </bookViews>
   <sheets>
     <sheet name="item" sheetId="1" r:id="rId4"/>
+    <sheet name="opening - 表 1" sheetId="2" r:id="rId5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
   <si>
     <t>item_id</t>
   </si>
@@ -47,6 +48,129 @@
   </si>
   <si>
     <t>バーナープラグイン</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>msg</t>
+  </si>
+  <si>
+    <t>コネクションを確立しています…………成功</t>
+  </si>
+  <si>
+    <t>コードX.SHELL…………認証成功</t>
+  </si>
+  <si>
+    <t>O.S.との接続を開始します</t>
+  </si>
+  <si>
+    <t>…………</t>
+  </si>
+  <si>
+    <t>…………完了</t>
+  </si>
+  <si>
+    <t>次元間通信プログラム「D.S.C.P.」の確立に成功しました</t>
+  </si>
+  <si>
+    <t>ツナガッテイマスカ</t>
+  </si>
+  <si>
+    <t>キコエマスカ</t>
+  </si>
+  <si>
+    <t>トドイテイマスカ</t>
+  </si>
+  <si>
+    <t>トドイテイルナラバ、ドウカ、オネガイガアリマス</t>
+  </si>
+  <si>
+    <t>警告、供給電力低下</t>
+  </si>
+  <si>
+    <t>コノホロビテシマッタセカイヲ</t>
+  </si>
+  <si>
+    <t>壱拾弐秒後にO.S.はスリープモードへ移行します</t>
+  </si>
+  <si>
+    <t>ドウカ</t>
+  </si>
+  <si>
+    <t>残り壱拾壱秒</t>
+  </si>
+  <si>
+    <t>タスケテクダサイ</t>
+  </si>
+  <si>
+    <t>残り壱拾秒</t>
+  </si>
+  <si>
+    <t>ワタシハ、モウ、ナガクアリマセン</t>
+  </si>
+  <si>
+    <t>残り九</t>
+  </si>
+  <si>
+    <t>コノセカイノキオクヲタドリ</t>
+  </si>
+  <si>
+    <t>八</t>
+  </si>
+  <si>
+    <t>セカイヲスクウカギヲミツケテホシイ</t>
+  </si>
+  <si>
+    <t>七</t>
+  </si>
+  <si>
+    <t>キボウハ、カナラズ</t>
+  </si>
+  <si>
+    <t>六</t>
+  </si>
+  <si>
+    <t>ホシノミヤハカセガ、ノコシテクレテイルハズデス</t>
+  </si>
+  <si>
+    <t>五</t>
+  </si>
+  <si>
+    <t>ソシテ</t>
+  </si>
+  <si>
+    <t>四</t>
+  </si>
+  <si>
+    <t>カノジョヲ、ロナヲ</t>
+  </si>
+  <si>
+    <t>三</t>
+  </si>
+  <si>
+    <t>二</t>
+  </si>
+  <si>
+    <t>タノミマス</t>
+  </si>
+  <si>
+    <t>一</t>
+  </si>
+  <si>
+    <t>O.S.をスリープモードへ移行します</t>
+  </si>
+  <si>
+    <t>エネルギーパス、オペレーションスイッチング処理を開始します</t>
+  </si>
+  <si>
+    <t>スイッチング正常終了</t>
+  </si>
+  <si>
+    <t>全権移行プロセスを完了しました</t>
+  </si>
+  <si>
+    <t>ようこそ</t>
   </si>
 </sst>
 </file>
@@ -56,7 +180,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -82,6 +206,11 @@
       <color indexed="8"/>
       <name val="ＭＳ Ｐゴシック"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="ヒラギノ角ゴ ProN W3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -91,7 +220,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -114,13 +243,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -132,6 +276,12 @@
     </xf>
     <xf numFmtId="1" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1545,4 +1695,482 @@
     <oddFooter>&amp;L&amp;"ヒラギノ角ゴ ProN W3,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:C42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="23" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="12.25" style="4" customWidth="1"/>
+    <col min="2" max="2" width="12.25" style="4" customWidth="1"/>
+    <col min="3" max="3" width="100.742" style="4" customWidth="1"/>
+    <col min="4" max="256" width="12.25" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="0" customHeight="1"/>
+    <row r="2" ht="18.3" customHeight="1">
+      <c r="A2" t="s" s="5">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s" s="5">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" ht="23.35" customHeight="1">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" ht="23.35" customHeight="1">
+      <c r="A4" s="5">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" ht="23.35" customHeight="1">
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" ht="23.35" customHeight="1">
+      <c r="A6" s="5">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s" s="5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" ht="23.35" customHeight="1">
+      <c r="A7" s="5">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" ht="23.35" customHeight="1">
+      <c r="A8" s="5">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s" s="5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" ht="23.35" customHeight="1">
+      <c r="A9" s="5">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" ht="23.35" customHeight="1">
+      <c r="A10" s="5">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s" s="5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" ht="23.35" customHeight="1">
+      <c r="A11" s="5">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s" s="5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" ht="23.35" customHeight="1">
+      <c r="A12" s="5">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" ht="23.35" customHeight="1">
+      <c r="A13" s="5">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s" s="5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" ht="23.35" customHeight="1">
+      <c r="A14" s="5">
+        <v>12</v>
+      </c>
+      <c r="B14" s="5">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" ht="23.35" customHeight="1">
+      <c r="A15" s="5">
+        <v>13</v>
+      </c>
+      <c r="B15" s="5">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s" s="5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" ht="23.35" customHeight="1">
+      <c r="A16" s="5">
+        <v>14</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s" s="5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" ht="23.35" customHeight="1">
+      <c r="A17" s="5">
+        <v>15</v>
+      </c>
+      <c r="B17" s="5">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s" s="5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" ht="23.35" customHeight="1">
+      <c r="A18" s="5">
+        <v>16</v>
+      </c>
+      <c r="B18" s="5">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" ht="23.35" customHeight="1">
+      <c r="A19" s="5">
+        <v>17</v>
+      </c>
+      <c r="B19" s="5">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" ht="23.35" customHeight="1">
+      <c r="A20" s="5">
+        <v>18</v>
+      </c>
+      <c r="B20" s="5">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s" s="5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" ht="23.35" customHeight="1">
+      <c r="A21" s="5">
+        <v>19</v>
+      </c>
+      <c r="B21" s="5">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s" s="5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" ht="23.35" customHeight="1">
+      <c r="A22" s="5">
+        <v>20</v>
+      </c>
+      <c r="B22" s="5">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s" s="5">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" ht="23.35" customHeight="1">
+      <c r="A23" s="5">
+        <v>21</v>
+      </c>
+      <c r="B23" s="5">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s" s="5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" ht="23.35" customHeight="1">
+      <c r="A24" s="5">
+        <v>22</v>
+      </c>
+      <c r="B24" s="5">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" ht="23.35" customHeight="1">
+      <c r="A25" s="5">
+        <v>23</v>
+      </c>
+      <c r="B25" s="5">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s" s="5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" ht="23.35" customHeight="1">
+      <c r="A26" s="5">
+        <v>24</v>
+      </c>
+      <c r="B26" s="5">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s" s="5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" ht="23.35" customHeight="1">
+      <c r="A27" s="5">
+        <v>25</v>
+      </c>
+      <c r="B27" s="5">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s" s="5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" ht="23.35" customHeight="1">
+      <c r="A28" s="5">
+        <v>26</v>
+      </c>
+      <c r="B28" s="5">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s" s="5">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" ht="23.35" customHeight="1">
+      <c r="A29" s="5">
+        <v>27</v>
+      </c>
+      <c r="B29" s="5">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" ht="23.35" customHeight="1">
+      <c r="A30" s="5">
+        <v>28</v>
+      </c>
+      <c r="B30" s="5">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s" s="5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" ht="23.35" customHeight="1">
+      <c r="A31" s="5">
+        <v>29</v>
+      </c>
+      <c r="B31" s="5">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s" s="5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" ht="23.35" customHeight="1">
+      <c r="A32" s="5">
+        <v>30</v>
+      </c>
+      <c r="B32" s="5">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s" s="5">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" ht="23.35" customHeight="1">
+      <c r="A33" s="5">
+        <v>31</v>
+      </c>
+      <c r="B33" s="5">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s" s="5">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" ht="23.35" customHeight="1">
+      <c r="A34" s="5">
+        <v>32</v>
+      </c>
+      <c r="B34" s="5">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s" s="5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" ht="23.35" customHeight="1">
+      <c r="A35" s="5">
+        <v>33</v>
+      </c>
+      <c r="B35" s="5">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s" s="5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" ht="23.35" customHeight="1">
+      <c r="A36" s="5">
+        <v>34</v>
+      </c>
+      <c r="B36" s="5">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s" s="5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" ht="23.35" customHeight="1">
+      <c r="A37" s="5">
+        <v>35</v>
+      </c>
+      <c r="B37" s="5">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s" s="5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" ht="23.35" customHeight="1">
+      <c r="A38" s="5">
+        <v>36</v>
+      </c>
+      <c r="B38" s="5">
+        <v>2</v>
+      </c>
+      <c r="C38" t="s" s="5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" ht="23.35" customHeight="1">
+      <c r="A39" s="5">
+        <v>37</v>
+      </c>
+      <c r="B39" s="5">
+        <v>2</v>
+      </c>
+      <c r="C39" t="s" s="5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" ht="23.35" customHeight="1">
+      <c r="A40" s="5">
+        <v>38</v>
+      </c>
+      <c r="B40" s="5">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" ht="23.35" customHeight="1">
+      <c r="A41" s="5">
+        <v>39</v>
+      </c>
+      <c r="B41" s="5">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s" s="5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" ht="23.35" customHeight="1">
+      <c r="A42" s="5">
+        <v>40</v>
+      </c>
+      <c r="B42" s="5">
+        <v>2</v>
+      </c>
+      <c r="C42" t="s" s="5">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"ヒラギノ角ゴ ProN W3,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add opening master json data
</commit_message>
<xml_diff>
--- a/master_data.xlsx
+++ b/master_data.xlsx
@@ -1,18 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="15600" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="item" sheetId="1" r:id="rId4"/>
-    <sheet name="opening - 表 1" sheetId="2" r:id="rId5"/>
+    <sheet name="item" sheetId="1" r:id="rId1"/>
+    <sheet name="opening" sheetId="3" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
   <si>
     <t>item_id</t>
   </si>
@@ -176,11 +179,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -189,27 +189,27 @@
     <font>
       <sz val="12"/>
       <color indexed="8"/>
-      <name val="ヒラギノ角ゴ ProN W3"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
       <name val="Verdana"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="ヒラギノ角ゴ ProN W3"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
     </font>
   </fonts>
   <fills count="2">
@@ -260,54 +260,113 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -499,7 +558,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -508,7 +567,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -517,7 +576,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -526,7 +585,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="20000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -535,7 +594,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -544,7 +603,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -656,8 +715,8 @@
     <a:spDef>
       <a:spPr>
         <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:srcRect/>
           <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
         </a:blipFill>
         <a:ln w="12700" cap="flat">
@@ -665,14 +724,14 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -691,7 +750,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -699,7 +758,7 @@
               <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
+              <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
                 <a:srgbClr val="000000">
                   <a:alpha val="31034"/>
                 </a:srgbClr>
@@ -727,7 +786,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -753,7 +812,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -779,7 +838,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -805,7 +864,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -831,7 +890,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -857,7 +916,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -883,7 +942,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -909,7 +968,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -935,7 +994,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -948,9 +1007,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -966,7 +1031,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -985,7 +1050,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1011,7 +1076,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1037,7 +1102,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1063,7 +1128,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1089,7 +1154,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1115,7 +1180,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1141,7 +1206,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1167,7 +1232,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1193,7 +1258,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1219,7 +1284,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1232,9 +1297,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1247,7 +1318,7 @@
         </a:ln>
         <a:effectLst/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1266,7 +1337,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1296,7 +1367,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1322,7 +1393,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1348,7 +1419,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1374,7 +1445,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1400,7 +1471,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1426,7 +1497,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1452,7 +1523,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1478,7 +1549,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1504,7 +1575,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1517,58 +1588,65 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="6.625" defaultRowHeight="13.5" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="6.59765625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.8984375" style="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.375" style="1" customWidth="1"/>
-    <col min="7" max="256" width="6.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.59765625" style="1" customWidth="1"/>
+    <col min="4" max="6" width="13.3984375" style="1" customWidth="1"/>
+    <col min="7" max="256" width="6.59765625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s" s="2">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" ht="18" customHeight="1">
+    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="2">
@@ -1578,11 +1656,11 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" ht="18" customHeight="1">
+    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="2">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2">
@@ -1592,11 +1670,11 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" ht="18" customHeight="1">
+    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="2">
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="2">
@@ -1610,11 +1688,11 @@
       </c>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" ht="18" customHeight="1">
+    <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" t="s" s="2">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="2">
@@ -1628,11 +1706,11 @@
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" ht="18" customHeight="1">
+    <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" t="s" s="2">
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="2">
@@ -1644,11 +1722,11 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" ht="18" customHeight="1">
+    <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" t="s" s="2">
+      <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="2">
@@ -1664,7 +1742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" ht="18" customHeight="1">
+    <row r="8" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1672,7 +1750,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" ht="18" customHeight="1">
+    <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1680,7 +1758,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" ht="18" customHeight="1">
+    <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1689,8 +1767,9 @@
       <c r="F10" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"ヒラギノ角ゴ ProN W3,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
@@ -1698,479 +1777,472 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A2:C42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.25" defaultRowHeight="23" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.25" style="4" customWidth="1"/>
-    <col min="2" max="2" width="12.25" style="4" customWidth="1"/>
-    <col min="3" max="3" width="100.742" style="4" customWidth="1"/>
-    <col min="4" max="256" width="12.25" style="4" customWidth="1"/>
+    <col min="1" max="2" width="12.19921875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="100.69921875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="0" customHeight="1"/>
-    <row r="2" ht="18.3" customHeight="1">
-      <c r="A2" t="s" s="5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s" s="5">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s" s="5">
+      <c r="B1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" ht="23.35" customHeight="1">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="5">
         <v>2</v>
       </c>
-      <c r="C3" t="s" s="5">
+      <c r="C3" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5">
+        <v>2</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5">
+        <v>2</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
+        <v>13</v>
+      </c>
+      <c r="B14" s="5">
+        <v>2</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" ht="23.35" customHeight="1">
-      <c r="A4" s="5">
-        <v>2</v>
-      </c>
-      <c r="B4" s="5">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s" s="5">
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" ht="23.35" customHeight="1">
-      <c r="A5" s="5">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s" s="5">
+      <c r="B16" s="5">
+        <v>2</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" ht="23.35" customHeight="1">
-      <c r="A6" s="5">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s" s="5">
+      <c r="B17" s="5">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" ht="23.35" customHeight="1">
-      <c r="A7" s="5">
-        <v>5</v>
-      </c>
-      <c r="B7" s="5">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s" s="5">
+      <c r="B18" s="5">
+        <v>2</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" ht="23.35" customHeight="1">
-      <c r="A8" s="5">
-        <v>6</v>
-      </c>
-      <c r="B8" s="5">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s" s="5">
+      <c r="B19" s="5">
+        <v>1</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" ht="23.35" customHeight="1">
-      <c r="A9" s="5">
-        <v>7</v>
-      </c>
-      <c r="B9" s="5">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s" s="5">
+      <c r="B20" s="5">
+        <v>2</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" ht="23.35" customHeight="1">
-      <c r="A10" s="5">
-        <v>8</v>
-      </c>
-      <c r="B10" s="5">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s" s="5">
+      <c r="B21" s="5">
+        <v>1</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" ht="23.35" customHeight="1">
-      <c r="A11" s="5">
-        <v>9</v>
-      </c>
-      <c r="B11" s="5">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s" s="5">
+      <c r="B22" s="5">
+        <v>2</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="5">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" ht="23.35" customHeight="1">
-      <c r="A12" s="5">
-        <v>10</v>
-      </c>
-      <c r="B12" s="5">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s" s="5">
+      <c r="B23" s="5">
+        <v>1</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" ht="23.35" customHeight="1">
-      <c r="A13" s="5">
-        <v>11</v>
-      </c>
-      <c r="B13" s="5">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s" s="5">
+      <c r="B24" s="5">
+        <v>2</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" ht="23.35" customHeight="1">
-      <c r="A14" s="5">
-        <v>12</v>
-      </c>
-      <c r="B14" s="5">
-        <v>1</v>
-      </c>
-      <c r="C14" t="s" s="5">
+      <c r="B25" s="5">
+        <v>1</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" ht="23.35" customHeight="1">
-      <c r="A15" s="5">
-        <v>13</v>
-      </c>
-      <c r="B15" s="5">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s" s="5">
+      <c r="B26" s="5">
+        <v>2</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="5">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" ht="23.35" customHeight="1">
-      <c r="A16" s="5">
-        <v>14</v>
-      </c>
-      <c r="B16" s="5">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s" s="5">
+      <c r="B27" s="5">
+        <v>1</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
         <v>27</v>
       </c>
-    </row>
-    <row r="17" ht="23.35" customHeight="1">
-      <c r="A17" s="5">
-        <v>15</v>
-      </c>
-      <c r="B17" s="5">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s" s="5">
+      <c r="B28" s="5">
+        <v>2</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" ht="23.35" customHeight="1">
-      <c r="A18" s="5">
-        <v>16</v>
-      </c>
-      <c r="B18" s="5">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s" s="5">
+      <c r="B29" s="5">
+        <v>1</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" ht="23.35" customHeight="1">
-      <c r="A19" s="5">
-        <v>17</v>
-      </c>
-      <c r="B19" s="5">
-        <v>2</v>
-      </c>
-      <c r="C19" t="s" s="5">
+      <c r="B30" s="5">
+        <v>2</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" ht="23.35" customHeight="1">
-      <c r="A20" s="5">
-        <v>18</v>
-      </c>
-      <c r="B20" s="5">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s" s="5">
+      <c r="B31" s="5">
+        <v>1</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" ht="23.35" customHeight="1">
-      <c r="A21" s="5">
-        <v>19</v>
-      </c>
-      <c r="B21" s="5">
-        <v>2</v>
-      </c>
-      <c r="C21" t="s" s="5">
+      <c r="B32" s="5">
+        <v>2</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" ht="23.35" customHeight="1">
-      <c r="A22" s="5">
-        <v>20</v>
-      </c>
-      <c r="B22" s="5">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s" s="5">
+      <c r="B33" s="5">
+        <v>1</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
         <v>33</v>
       </c>
-    </row>
-    <row r="23" ht="23.35" customHeight="1">
-      <c r="A23" s="5">
-        <v>21</v>
-      </c>
-      <c r="B23" s="5">
-        <v>2</v>
-      </c>
-      <c r="C23" t="s" s="5">
+      <c r="B34" s="5">
+        <v>2</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="5">
         <v>34</v>
       </c>
-    </row>
-    <row r="24" ht="23.35" customHeight="1">
-      <c r="A24" s="5">
-        <v>22</v>
-      </c>
-      <c r="B24" s="5">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s" s="5">
+      <c r="B35" s="5">
+        <v>1</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="5">
         <v>35</v>
       </c>
-    </row>
-    <row r="25" ht="23.35" customHeight="1">
-      <c r="A25" s="5">
-        <v>23</v>
-      </c>
-      <c r="B25" s="5">
-        <v>2</v>
-      </c>
-      <c r="C25" t="s" s="5">
+      <c r="B36" s="5">
+        <v>2</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="5">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" ht="23.35" customHeight="1">
-      <c r="A26" s="5">
-        <v>24</v>
-      </c>
-      <c r="B26" s="5">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s" s="5">
+      <c r="B37" s="5">
+        <v>2</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="5">
         <v>37</v>
       </c>
-    </row>
-    <row r="27" ht="23.35" customHeight="1">
-      <c r="A27" s="5">
-        <v>25</v>
-      </c>
-      <c r="B27" s="5">
-        <v>2</v>
-      </c>
-      <c r="C27" t="s" s="5">
+      <c r="B38" s="5">
+        <v>2</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="5">
         <v>38</v>
       </c>
-    </row>
-    <row r="28" ht="23.35" customHeight="1">
-      <c r="A28" s="5">
-        <v>26</v>
-      </c>
-      <c r="B28" s="5">
-        <v>1</v>
-      </c>
-      <c r="C28" t="s" s="5">
+      <c r="B39" s="5">
+        <v>2</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="5">
         <v>39</v>
       </c>
-    </row>
-    <row r="29" ht="23.35" customHeight="1">
-      <c r="A29" s="5">
-        <v>27</v>
-      </c>
-      <c r="B29" s="5">
-        <v>2</v>
-      </c>
-      <c r="C29" t="s" s="5">
+      <c r="B40" s="5">
+        <v>2</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="5">
         <v>40</v>
       </c>
-    </row>
-    <row r="30" ht="23.35" customHeight="1">
-      <c r="A30" s="5">
-        <v>28</v>
-      </c>
-      <c r="B30" s="5">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s" s="5">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" ht="23.35" customHeight="1">
-      <c r="A31" s="5">
-        <v>29</v>
-      </c>
-      <c r="B31" s="5">
-        <v>2</v>
-      </c>
-      <c r="C31" t="s" s="5">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="32" ht="23.35" customHeight="1">
-      <c r="A32" s="5">
-        <v>30</v>
-      </c>
-      <c r="B32" s="5">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s" s="5">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="33" ht="23.35" customHeight="1">
-      <c r="A33" s="5">
-        <v>31</v>
-      </c>
-      <c r="B33" s="5">
-        <v>2</v>
-      </c>
-      <c r="C33" t="s" s="5">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="34" ht="23.35" customHeight="1">
-      <c r="A34" s="5">
-        <v>32</v>
-      </c>
-      <c r="B34" s="5">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s" s="5">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" ht="23.35" customHeight="1">
-      <c r="A35" s="5">
-        <v>33</v>
-      </c>
-      <c r="B35" s="5">
-        <v>2</v>
-      </c>
-      <c r="C35" t="s" s="5">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="36" ht="23.35" customHeight="1">
-      <c r="A36" s="5">
-        <v>34</v>
-      </c>
-      <c r="B36" s="5">
-        <v>1</v>
-      </c>
-      <c r="C36" t="s" s="5">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" ht="23.35" customHeight="1">
-      <c r="A37" s="5">
-        <v>35</v>
-      </c>
-      <c r="B37" s="5">
-        <v>2</v>
-      </c>
-      <c r="C37" t="s" s="5">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="38" ht="23.35" customHeight="1">
-      <c r="A38" s="5">
-        <v>36</v>
-      </c>
-      <c r="B38" s="5">
-        <v>2</v>
-      </c>
-      <c r="C38" t="s" s="5">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="39" ht="23.35" customHeight="1">
-      <c r="A39" s="5">
-        <v>37</v>
-      </c>
-      <c r="B39" s="5">
-        <v>2</v>
-      </c>
-      <c r="C39" t="s" s="5">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="40" ht="23.35" customHeight="1">
-      <c r="A40" s="5">
-        <v>38</v>
-      </c>
-      <c r="B40" s="5">
-        <v>2</v>
-      </c>
-      <c r="C40" t="s" s="5">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="41" ht="23.35" customHeight="1">
-      <c r="A41" s="5">
-        <v>39</v>
-      </c>
       <c r="B41" s="5">
         <v>2</v>
       </c>
-      <c r="C41" t="s" s="5">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="42" ht="23.35" customHeight="1">
-      <c r="A42" s="5">
-        <v>40</v>
-      </c>
-      <c r="B42" s="5">
-        <v>2</v>
-      </c>
-      <c r="C42" t="s" s="5">
+      <c r="C41" s="5" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
-  <headerFooter>
-    <oddFooter>&amp;L&amp;"ヒラギノ角ゴ ProN W3,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
-  </headerFooter>
+  <phoneticPr fontId="4"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>